<commit_message>
Output window for error outputs
</commit_message>
<xml_diff>
--- a/GanttChartPROG25.xlsx
+++ b/GanttChartPROG25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlandgraff\source\repos\prog1004-gruppe-25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E7BE1C-509D-4BE7-983F-86F3F5860C4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD69EB4-050E-42AD-A658-DF32EC0FDB28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{869F4D6E-3DCD-43F9-A693-0C5EA342B78F}"/>
   </bookViews>
@@ -616,7 +616,7 @@
   <dimension ref="A1:BV29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>